<commit_message>
Update to Kostenrechnung--Added Versions of different Hardware configurations-- PS:Abstimmung welche Version gewählt wird kommt, nach Gespräch mit HG via Discord
</commit_message>
<xml_diff>
--- a/Diplomarbeit/doc/Kostenrechnung_Hardware.xlsx
+++ b/Diplomarbeit/doc/Kostenrechnung_Hardware.xlsx
@@ -5,12 +5,13 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\Diplomarbeit\Contrude\Diplomarbeit\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maximilian\Desktop\Contrude\Diplomarbeit\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9820F125-0312-48DA-BA5C-5A9CC00301E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07084B7-D81A-459C-812C-247892DB73E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{268A7986-C005-4251-90D6-2DE7661BB465}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{268A7986-C005-4251-90D6-2DE7661BB465}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="1" xr2:uid="{F8F58720-A04D-47BF-B44C-22AB8B67CE72}"/>
   </bookViews>
   <sheets>
     <sheet name="Anforderungen" sheetId="1" r:id="rId1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="52">
   <si>
     <t>Auflagen</t>
   </si>
@@ -87,9 +88,6 @@
     <t>Amazon</t>
   </si>
   <si>
-    <t>ICQUANZX GY-NEO6MV2 NEO-6M GPS Flight Control Module</t>
-  </si>
-  <si>
     <t>GY-NEO6MV2</t>
   </si>
   <si>
@@ -157,6 +155,45 @@
   </si>
   <si>
     <t>electronics Semaf</t>
+  </si>
+  <si>
+    <t>Gerät</t>
+  </si>
+  <si>
+    <t>Gesamtpreis</t>
+  </si>
+  <si>
+    <t>Preis / Stk (auch Preis pro Person)</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>VersionsNR</t>
+  </si>
+  <si>
+    <t>VersionsName</t>
+  </si>
+  <si>
+    <t>Billigste &amp; Komfortabelste Variante (mit Aliexpress)</t>
+  </si>
+  <si>
+    <t>Billigste &amp; Komfortabelste Variante (ohne Aliexpress)</t>
+  </si>
+  <si>
+    <t>Raspberry Zero Variante  (mit Aliexpress)</t>
+  </si>
+  <si>
+    <t>Arduino Nano Variante  (mit Aliexpress)</t>
+  </si>
+  <si>
+    <t>Raspberry Zero Variante  (ohen Aliexpress)</t>
+  </si>
+  <si>
+    <t>Arduino Nano Variante  (ohen Aliexpress)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GY-NEO6MV2 Flight Control Module</t>
   </si>
 </sst>
 </file>
@@ -213,7 +250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +269,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -306,13 +355,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -325,6 +428,13 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -334,15 +444,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Link" xfId="2" builtinId="8"/>
@@ -682,16 +794,17 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" style="10" bestFit="1" customWidth="1"/>
@@ -702,18 +815,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="14"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="2:11" ht="24" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
@@ -762,22 +875,22 @@
         <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="8">
         <v>16.5</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="8">
         <v>29.75</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -785,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6">
         <v>9.06</v>
@@ -794,22 +907,22 @@
         <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="8">
         <v>1.1100000000000001</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="8">
         <v>50</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -817,63 +930,63 @@
         <v>2</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="6">
         <v>1.6</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="8">
         <v>0.25</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" s="6">
         <v>5.9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
+      <c r="C7" s="32" t="s">
+        <v>25</v>
       </c>
       <c r="D7" s="6">
-        <v>6.44</v>
+        <v>3.02</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="G7" s="8">
         <v>10.130000000000001</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" s="6">
         <v>5.9</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -881,31 +994,31 @@
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="6">
         <v>3.99</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="8">
         <v>2.72</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="6">
         <v>6.5</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -913,31 +1026,31 @@
         <v>5</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6">
         <v>3.79</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="8">
         <v>10.01</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="6">
         <v>5.9</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -948,100 +1061,74 @@
       <c r="D12" s="11"/>
     </row>
     <row r="13" spans="2:11" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
     </row>
     <row r="14" spans="2:11" ht="24" x14ac:dyDescent="0.4">
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="15"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="21"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="21"/>
-    </row>
-    <row r="17" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="21"/>
-    </row>
-    <row r="18" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="21"/>
-    </row>
-    <row r="19" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="21"/>
-    </row>
-    <row r="20" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="21"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="I16" s="16"/>
+    </row>
+    <row r="17" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="F19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1049,23 +1136,23 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{B1628E4A-1DB5-40B9-9995-39F8B7BB1A93}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{4A34D5EA-7C2E-48C2-8CFC-665118B8C054}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{9B63FE35-81FB-48E8-9BDA-B76D1DF70B58}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{7B831A91-4041-4AF0-8989-FE70C24EE7FC}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{F092B410-15C3-4922-90B4-6AD51D30F69E}"/>
-    <hyperlink ref="I6" r:id="rId6" xr:uid="{3DE3E015-F5DE-4A42-9951-4A815CCEB2B0}"/>
-    <hyperlink ref="I7" r:id="rId7" xr:uid="{EDB4D6B5-5B05-403A-B34C-64244A49BECF}"/>
-    <hyperlink ref="I9" r:id="rId8" xr:uid="{D78F8166-EB4B-45CD-BA0A-FC9AE20E92AF}"/>
-    <hyperlink ref="F6" r:id="rId9" xr:uid="{4ABE941E-E49C-4B82-8380-FBEECA044211}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{8D9A7036-7E08-459F-B412-DBDB4CC2B3E2}"/>
-    <hyperlink ref="F7" r:id="rId11" xr:uid="{34F0DC53-5B0E-4131-B527-0ED4A343448B}"/>
-    <hyperlink ref="C9" r:id="rId12" xr:uid="{81F15471-C69D-490D-ABF6-CAFD9C89C6BE}"/>
-    <hyperlink ref="C8" r:id="rId13" xr:uid="{7E21618D-F8CD-488E-834F-0432447306C9}"/>
-    <hyperlink ref="F8" r:id="rId14" xr:uid="{0BFCB48E-6BD1-4D70-BCEE-5D66482D3C30}"/>
-    <hyperlink ref="F9" r:id="rId15" xr:uid="{E0FF6279-CBF7-49A3-A5C5-F406D2786A3B}"/>
-    <hyperlink ref="I4" r:id="rId16" xr:uid="{8FF065F6-6846-4DD0-B759-38337B417B47}"/>
-    <hyperlink ref="I5" r:id="rId17" xr:uid="{5926A4B2-0BF5-41A4-89C1-F66AA8B8250F}"/>
-    <hyperlink ref="I8" r:id="rId18" xr:uid="{6F8AE5B9-5B77-4EB1-BF90-6BAC815576C5}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{9B63FE35-81FB-48E8-9BDA-B76D1DF70B58}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{7B831A91-4041-4AF0-8989-FE70C24EE7FC}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{F092B410-15C3-4922-90B4-6AD51D30F69E}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{3DE3E015-F5DE-4A42-9951-4A815CCEB2B0}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{EDB4D6B5-5B05-403A-B34C-64244A49BECF}"/>
+    <hyperlink ref="I9" r:id="rId7" xr:uid="{D78F8166-EB4B-45CD-BA0A-FC9AE20E92AF}"/>
+    <hyperlink ref="F6" r:id="rId8" xr:uid="{4ABE941E-E49C-4B82-8380-FBEECA044211}"/>
+    <hyperlink ref="F7" r:id="rId9" xr:uid="{34F0DC53-5B0E-4131-B527-0ED4A343448B}"/>
+    <hyperlink ref="C9" r:id="rId10" xr:uid="{81F15471-C69D-490D-ABF6-CAFD9C89C6BE}"/>
+    <hyperlink ref="C8" r:id="rId11" xr:uid="{7E21618D-F8CD-488E-834F-0432447306C9}"/>
+    <hyperlink ref="F8" r:id="rId12" xr:uid="{0BFCB48E-6BD1-4D70-BCEE-5D66482D3C30}"/>
+    <hyperlink ref="F9" r:id="rId13" xr:uid="{E0FF6279-CBF7-49A3-A5C5-F406D2786A3B}"/>
+    <hyperlink ref="I4" r:id="rId14" xr:uid="{8FF065F6-6846-4DD0-B759-38337B417B47}"/>
+    <hyperlink ref="I5" r:id="rId15" xr:uid="{5926A4B2-0BF5-41A4-89C1-F66AA8B8250F}"/>
+    <hyperlink ref="I8" r:id="rId16" xr:uid="{6F8AE5B9-5B77-4EB1-BF90-6BAC815576C5}"/>
+    <hyperlink ref="C5" r:id="rId17" display="ICQUANZX GY-NEO6MV2 NEO-6M GPS Flight Control Module" xr:uid="{6E83B416-8461-482D-8139-C01525CFDB5B}"/>
+    <hyperlink ref="C7" r:id="rId18" xr:uid="{8F2300DB-EC22-44B9-8D00-B2AEED4BA31F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1074,18 +1161,23 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3EDCA9-5D91-4A92-B956-2E6486458450}">
   <sheetPr codeName="Tabelle4"/>
-  <dimension ref="A1"/>
+  <dimension ref="B1:XFD43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="1">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="25" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
@@ -1100,7 +1192,458 @@
     <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B1" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6">
+        <f xml:space="preserve"> 9.9+3.99</f>
+        <v>13.89</v>
+      </c>
+      <c r="XFD3" s="10">
+        <f>SUM(E3:XFC3)</f>
+        <v>13.89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="XFD4" s="10">
+        <f>SUM(E4:XFC4)</f>
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2.72</v>
+      </c>
+      <c r="XFD5" s="10">
+        <f>SUM(E5:XFC5)</f>
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5.9</v>
+      </c>
+      <c r="XFD6" s="10">
+        <f>SUM(E6:XFC6)</f>
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5 16384:16384" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="8">
+        <f>SUM(E3:E6)</f>
+        <v>23.619999999999997</v>
+      </c>
+      <c r="XFD7" s="10">
+        <f>SUM(E7:XFC7)</f>
+        <v>23.619999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D8" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="8">
+        <f>E7*3</f>
+        <v>70.859999999999985</v>
+      </c>
+      <c r="XFD8" s="10">
+        <f>SUM(E8:XFC8)</f>
+        <v>70.859999999999985</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="24"/>
+      <c r="D10" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="6">
+        <f xml:space="preserve"> 9.9+3.99</f>
+        <v>13.89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="6">
+        <v>9.06</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5 16384:16384" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="6">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5 16384:16384" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="8">
+        <f>SUM(E10:E13)</f>
+        <v>31.57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
+      <c r="D15" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="8">
+        <f>E14*3</f>
+        <v>94.710000000000008</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5 16384:16384" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="8">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="6">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="8">
+        <f>SUM(E17:E20)</f>
+        <v>26.229999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="8">
+        <f>E21*3</f>
+        <v>78.69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="8">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="6">
+        <v>9.06</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="8">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="6">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="8">
+        <f>SUM(E24:E27)</f>
+        <v>34.18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="8">
+        <f>E28*3</f>
+        <v>102.53999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>5</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="8">
+        <v>29.75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="8">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="8">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="6">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" s="8">
+        <f>SUM(E31:E34)</f>
+        <v>39.479999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="8">
+        <f>E35*3</f>
+        <v>118.44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>6</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="8">
+        <v>29.75</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="6">
+        <v>9.06</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="8">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" s="6">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="8">
+        <f>SUM(E38:E41)</f>
+        <v>47.43</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E43" s="8">
+        <f>E42*3</f>
+        <v>142.29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{F7947900-EFA9-4457-B494-EDF23B53B7AE}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{421027E6-7C62-4692-A583-385851416151}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{7BA684F6-A8E9-4E3D-91B4-089C1774CF50}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{5847FB82-5364-4CD3-AF3C-55448CA22714}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{936A9F46-1262-4185-AADB-24149FEEC9A9}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{E5FB7CAC-E27A-4B67-97CD-0765074F0C70}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{6EEAA285-1B1C-47E3-B374-3EC13CA699A9}"/>
+    <hyperlink ref="D18" r:id="rId8" xr:uid="{540CF053-3BF8-427E-9971-0C2945DBAFBB}"/>
+    <hyperlink ref="D19" r:id="rId9" xr:uid="{11709238-88D3-4122-ADF5-D4F7D170C749}"/>
+    <hyperlink ref="D20" r:id="rId10" xr:uid="{51B2FF76-F49B-4282-A8D7-2BEE8130D84A}"/>
+    <hyperlink ref="D17" r:id="rId11" xr:uid="{EF98E5CC-65E1-45F6-9129-F8740517FF9A}"/>
+    <hyperlink ref="D26" r:id="rId12" xr:uid="{416232F3-637E-4FDE-ADB2-F89E032A69F0}"/>
+    <hyperlink ref="D27" r:id="rId13" xr:uid="{9C4F8C2D-B60D-4A26-8E10-638B107343AC}"/>
+    <hyperlink ref="D24" r:id="rId14" xr:uid="{9E663B94-D129-47B0-8750-154647918595}"/>
+    <hyperlink ref="D33" r:id="rId15" xr:uid="{AFA75890-9FEB-4A5C-BBA9-3E84E2F22867}"/>
+    <hyperlink ref="D34" r:id="rId16" xr:uid="{DB8332AA-3228-4DB1-9BBD-6A3DE5BAF400}"/>
+    <hyperlink ref="D40" r:id="rId17" xr:uid="{F5702130-8237-4848-AFEC-6998DDC23AF8}"/>
+    <hyperlink ref="D41" r:id="rId18" xr:uid="{177A6186-5F3A-4AEE-8B0D-2738FE0ADC74}"/>
+    <hyperlink ref="D39" r:id="rId19" display="ICQUANZX GY-NEO6MV2 NEO-6M GPS Flight Control Module" xr:uid="{460FEA35-0568-41D3-BF0D-AD982069BFEB}"/>
+    <hyperlink ref="D32" r:id="rId20" xr:uid="{B0BFBF8F-8ECA-415C-8635-EC11FDCA62AB}"/>
+    <hyperlink ref="D25" r:id="rId21" display="ICQUANZX GY-NEO6MV2 NEO-6M GPS Flight Control Module" xr:uid="{693D0D67-A738-4FBD-948C-39212A6FA339}"/>
+    <hyperlink ref="D11" r:id="rId22" display="ICQUANZX GY-NEO6MV2 NEO-6M GPS Flight Control Module" xr:uid="{E387F0D6-6A54-4668-A27B-DED65F7D3742}"/>
+    <hyperlink ref="D31" r:id="rId23" xr:uid="{338511E0-5744-4D6B-91B1-9B106E363D0A}"/>
+    <hyperlink ref="D38" r:id="rId24" xr:uid="{29EABC2A-35BD-4CAC-92EF-B9DF093D822A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>